<commit_message>
Added test case for Forgot Password and captured Registration objects
</commit_message>
<xml_diff>
--- a/target/classes/selenium/academy/testdata/LoginData.xlsx
+++ b/target/classes/selenium/academy/testdata/LoginData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmahe\eclipse-workspace\academy\src\main\java\selenium\academy\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{516949D1-D1F5-42AA-BAA2-67AC60948561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04804AB1-9AA7-40C7-BEA5-75E45F5FB0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{51E5687A-F001-4195-A7F5-07583581B3C2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -446,7 +446,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>